<commit_message>
Added more benchmark/result info
</commit_message>
<xml_diff>
--- a/figures/benchmark-data.xlsx
+++ b/figures/benchmark-data.xlsx
@@ -12,9 +12,9 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="cpp" localSheetId="0">Sheet1!$A$27:$G$32</definedName>
-    <definedName name="cpp_js_chrome" localSheetId="0">Sheet1!$A$36:$G$41</definedName>
-    <definedName name="js_chrome" localSheetId="0">Sheet1!$A$45:$D$50</definedName>
+    <definedName name="cpp" localSheetId="0">Sheet1!$A$30:$G$35</definedName>
+    <definedName name="cpp_js_chrome" localSheetId="0">Sheet1!$A$39:$G$44</definedName>
+    <definedName name="js_chrome" localSheetId="0">Sheet1!$A$48:$D$53</definedName>
     <definedName name="js_chrome" localSheetId="1">Sheet2!$A$2:$D$7</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="29">
   <si>
     <t>Benchmark</t>
   </si>
@@ -163,13 +163,13 @@
     <t>Emscripten Chrome</t>
   </si>
   <si>
-    <t>C++/Handwritten Chrome</t>
+    <t>AVERAGE</t>
   </si>
   <si>
-    <t>C++/Emscripten Chrome</t>
+    <t>JS Handwritten Chrome</t>
   </si>
   <si>
-    <t>C++/C++</t>
+    <t>JS Emscripten Chrome</t>
   </si>
 </sst>
 </file>
@@ -242,10 +242,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.6061232106974616E-2"/>
-          <c:y val="3.1099494916076668E-2"/>
-          <c:w val="0.89907572527414703"/>
-          <c:h val="0.72690175418720138"/>
+          <c:x val="8.2431459715445923E-2"/>
+          <c:y val="2.8590689321729514E-2"/>
+          <c:w val="0.8998967942200311"/>
+          <c:h val="0.76915905511811022"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -257,7 +257,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$1</c:f>
+              <c:f>Sheet1!$E$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -266,17 +266,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$20:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>AverageFloat32x4</c:v>
                 </c:pt>
@@ -294,33 +289,39 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MatrixInverse</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVERAGE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>Sheet1!$E$20:$E$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>4.07</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.78</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.66</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.53</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.96</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.27</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -331,11 +332,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$F$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Handwritten Chrome</c:v>
+                  <c:v>JS Handwritten Chrome</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -343,9 +344,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$20:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>AverageFloat32x4</c:v>
                 </c:pt>
@@ -363,33 +364,39 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MatrixInverse</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVERAGE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>Sheet1!$F$20:$F$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.8538812785388128</c:v>
+                  <c:v>0.95148986301369864</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7425373134328357</c:v>
+                  <c:v>0.9309250373134329</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8142857142857141</c:v>
+                  <c:v>0.75654835714285706</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.8518518518518516</c:v>
+                  <c:v>0.85589307407407411</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6489361702127661</c:v>
+                  <c:v>0.84628270212765966</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.1229508196721305</c:v>
+                  <c:v>0.89244019672131147</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8722632050655057</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -400,11 +407,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$G$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Emscripten Chrome</c:v>
+                  <c:v>JS Emscripten Chrome</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -412,9 +419,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$20:$A$26</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>AverageFloat32x4</c:v>
                 </c:pt>
@@ -432,33 +439,39 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MatrixInverse</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVERAGE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:f>Sheet1!$G$20:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.88</c:v>
+                  <c:v>0.80024968789013728</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.84</c:v>
+                  <c:v>0.91223404255319152</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.41</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.87</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.12</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.47</c:v>
+                  <c:v>0.59090909090909094</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.52278769244762546</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -473,11 +486,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="42339712"/>
-        <c:axId val="42357888"/>
+        <c:axId val="48260224"/>
+        <c:axId val="98265728"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="42339712"/>
+        <c:axId val="48260224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -491,12 +504,12 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" baseline="0"/>
+              <a:defRPr sz="1200"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="42357888"/>
+        <c:crossAx val="98265728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -504,7 +517,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42357888"/>
+        <c:axId val="98265728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,11 +531,19 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1200" baseline="0"/>
+                  <a:defRPr sz="1400"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1200" baseline="0"/>
-                  <a:t>SIMD/Scalar Speedup</a:t>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>SIMD C++ vs. JavaScript</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> relative performance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t> </a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -534,17 +555,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" baseline="0"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="42339712"/>
+        <c:crossAx val="48260224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -555,16 +566,13 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.16399567077250546"/>
-          <c:y val="0.14005602240896359"/>
-          <c:w val="0.70838687199498296"/>
-          <c:h val="5.4961574047848336E-2"/>
+          <c:x val="0.13046159574753782"/>
+          <c:y val="6.4561403508771931E-2"/>
+          <c:w val="0.79771385351328894"/>
+          <c:h val="4.8199747998335443E-2"/>
         </c:manualLayout>
       </c:layout>
-      <c:overlay val="1"/>
-      <c:spPr>
-        <a:noFill/>
-      </c:spPr>
+      <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
@@ -609,6 +617,391 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
+          <c:x val="7.6061232106974616E-2"/>
+          <c:y val="3.1099494916076668E-2"/>
+          <c:w val="0.89907572527414703"/>
+          <c:h val="0.72690175418720138"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>AverageFloat32x4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mandelbrot</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MatrixMultiplication</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VertexTransform</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MatrixTranspose</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MatrixInverse</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVERAGE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>4.07</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.78</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.66</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3783333333333334</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JS Handwritten Chrome</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>AverageFloat32x4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mandelbrot</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MatrixMultiplication</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VertexTransform</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MatrixTranspose</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MatrixInverse</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVERAGE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.8538812785388128</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7425373134328357</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8142857142857141</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.8518518518518516</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6489361702127661</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1229508196721305</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.6724071913323515</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>JS Emscripten Chrome</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>AverageFloat32x4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Mandelbrot</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>MatrixMultiplication</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>VertexTransform</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>MatrixTranspose</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>MatrixInverse</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVERAGE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.41</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.87</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.47</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5983333333333332</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="45712896"/>
+        <c:axId val="45714432"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="45712896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="45714432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="45714432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" baseline="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t>SIMD vs. Scalar relative performance</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="45712896"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17972824193435996"/>
+          <c:y val="4.173473819369701E-2"/>
+          <c:w val="0.70838687199498296"/>
+          <c:h val="5.4961574047848336E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:noFill/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" baseline="0"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
           <c:x val="8.2431459715445923E-2"/>
           <c:y val="2.8590689321729514E-2"/>
           <c:w val="0.8998967942200311"/>
@@ -628,7 +1021,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C++/C++</c:v>
+                  <c:v>C++</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -636,9 +1029,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$11:$A$16</c:f>
+              <c:f>Sheet1!$A$11:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>AverageFloat32x4</c:v>
                 </c:pt>
@@ -656,16 +1049,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MatrixInverse</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVERAGE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$11:$E$16</c:f>
+              <c:f>Sheet1!$E$11:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -682,6 +1078,9 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -697,7 +1096,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C++/Handwritten Chrome</c:v>
+                  <c:v>JS Handwritten Chrome</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -705,9 +1104,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$11:$A$16</c:f>
+              <c:f>Sheet1!$A$11:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>AverageFloat32x4</c:v>
                 </c:pt>
@@ -725,16 +1124,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MatrixInverse</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVERAGE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$11:$F$16</c:f>
+              <c:f>Sheet1!$F$11:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1.0048977725118484</c:v>
                 </c:pt>
@@ -752,6 +1154,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.36340458526740665</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.70746827108500243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -766,7 +1171,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>C++/Emscripten Chrome</c:v>
+                  <c:v>JS Emscripten Chrome</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -774,9 +1179,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$11:$A$16</c:f>
+              <c:f>Sheet1!$A$11:$A$17</c:f>
               <c:strCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>AverageFloat32x4</c:v>
                 </c:pt>
@@ -794,16 +1199,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>MatrixInverse</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>AVERAGE</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$11:$G$16</c:f>
+              <c:f>Sheet1!$G$11:$G$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.83872696099442778</c:v>
                 </c:pt>
@@ -821,6 +1229,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.29452054794520549</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.50988851671181712</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -835,11 +1246,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="83995264"/>
-        <c:axId val="98271616"/>
+        <c:axId val="45740800"/>
+        <c:axId val="45742336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="83995264"/>
+        <c:axId val="45740800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -858,7 +1269,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98271616"/>
+        <c:crossAx val="45742336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -866,7 +1277,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="98271616"/>
+        <c:axId val="45742336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -884,7 +1295,15 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Scalar speedup over C++ </a:t>
+                  <a:t>Scalar C++ vs. JavaScript</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> relative performance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t> </a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -896,7 +1315,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83995264"/>
+        <c:crossAx val="45740800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -941,21 +1360,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>161926</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>123826</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>109539</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -971,20 +1392,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>395286</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>266699</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>123824</xdr:rowOff>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -999,19 +1420,49 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>357187</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>533401</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="js-chrome" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cpp-js-chrome" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cpp-js-chrome" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cpp" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="cpp" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="js-chrome" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1305,10 +1756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="V24" sqref="V24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1330,10 +1781,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -1341,15 +1792,15 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <f>G27</f>
+        <f>G30</f>
         <v>4.07</v>
       </c>
       <c r="C2">
-        <f>D45/C45</f>
+        <f>D48/C48</f>
         <v>3.8538812785388128</v>
       </c>
       <c r="D2">
-        <f>G36</f>
+        <f>G39</f>
         <v>3.88</v>
       </c>
     </row>
@@ -1358,15 +1809,15 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B7" si="0">G28</f>
+        <f t="shared" ref="B3:B7" si="0">G31</f>
         <v>3.78</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C7" si="1">D46/C46</f>
+        <f t="shared" ref="C3:C7" si="1">D49/C49</f>
         <v>3.7425373134328357</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D7" si="2">G37</f>
+        <f t="shared" ref="D3:D7" si="2">G40</f>
         <v>4.84</v>
       </c>
     </row>
@@ -1438,6 +1889,23 @@
         <v>6.47</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(B2:B7)</f>
+        <v>3.3783333333333334</v>
+      </c>
+      <c r="C8">
+        <f>AVERAGE(C2:C7)</f>
+        <v>4.6724071913323515</v>
+      </c>
+      <c r="D8">
+        <f>AVERAGE(D2:D7)</f>
+        <v>3.5983333333333332</v>
+      </c>
+    </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
@@ -1452,13 +1920,13 @@
         <v>25</v>
       </c>
       <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" t="s">
         <v>28</v>
-      </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1466,15 +1934,15 @@
         <v>2</v>
       </c>
       <c r="B11">
-        <f>D27</f>
+        <f>D30</f>
         <v>7827</v>
       </c>
       <c r="C11">
-        <f>1000*1000*D45/B45</f>
+        <f>1000*1000*D48/B48</f>
         <v>7788.8519748984863</v>
       </c>
       <c r="D11">
-        <f>D36</f>
+        <f>D39</f>
         <v>9332</v>
       </c>
       <c r="E11">
@@ -1482,11 +1950,11 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <f>B11/C11</f>
+        <f t="shared" ref="F11:F16" si="3">B11/C11</f>
         <v>1.0048977725118484</v>
       </c>
       <c r="G11">
-        <f>B11/D11</f>
+        <f t="shared" ref="G11:G16" si="4">B11/D11</f>
         <v>0.83872696099442778</v>
       </c>
     </row>
@@ -1495,27 +1963,27 @@
         <v>3</v>
       </c>
       <c r="B12">
-        <f t="shared" ref="B12:B16" si="3">D28</f>
+        <f t="shared" ref="B12:B16" si="5">D31</f>
         <v>1298</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:C16" si="4">1000*1000*D46/B46</f>
+        <f t="shared" ref="C12:C16" si="6">1000*1000*D49/B49</f>
         <v>1378.9405666992041</v>
       </c>
       <c r="D12">
-        <f t="shared" ref="D12:D16" si="5">D37</f>
+        <f t="shared" ref="D12:D16" si="7">D40</f>
         <v>1824</v>
       </c>
       <c r="E12">
-        <f t="shared" ref="E12:E16" si="6">B12/B12</f>
+        <f t="shared" ref="E12:E16" si="8">B12/B12</f>
         <v>1</v>
       </c>
       <c r="F12">
-        <f>B12/C12</f>
+        <f t="shared" si="3"/>
         <v>0.94130235294117637</v>
       </c>
       <c r="G12">
-        <f>B12/D12</f>
+        <f t="shared" si="4"/>
         <v>0.71162280701754388</v>
       </c>
     </row>
@@ -1524,27 +1992,27 @@
         <v>4</v>
       </c>
       <c r="B13">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="6"/>
+        <v>31.817435520361883</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="7"/>
+        <v>36</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F13">
         <f t="shared" si="3"/>
-        <v>15</v>
-      </c>
-      <c r="C13">
+        <v>0.47143962908011872</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="4"/>
-        <v>31.817435520361883</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="5"/>
-        <v>36</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <f>B13/C13</f>
-        <v>0.47143962908011872</v>
-      </c>
-      <c r="G13">
-        <f>B13/D13</f>
         <v>0.41666666666666669</v>
       </c>
     </row>
@@ -1553,27 +2021,27 @@
         <v>5</v>
       </c>
       <c r="B14">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="6"/>
+        <v>9.0007781778556364</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F14">
         <f t="shared" si="3"/>
-        <v>9</v>
-      </c>
-      <c r="C14">
+        <v>0.99991354326923076</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="4"/>
-        <v>9.0007781778556364</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <f>B14/C14</f>
-        <v>0.99991354326923076</v>
-      </c>
-      <c r="G14">
-        <f>B14/D14</f>
         <v>0.5625</v>
       </c>
     </row>
@@ -1582,27 +2050,27 @@
         <v>6</v>
       </c>
       <c r="B15">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="6"/>
+        <v>8.6234450049348474</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F15">
         <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="C15">
+        <v>0.46385174344023328</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="4"/>
-        <v>8.6234450049348474</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <f>B15/C15</f>
-        <v>0.46385174344023328</v>
-      </c>
-      <c r="G15">
-        <f>B15/D15</f>
         <v>0.23529411764705882</v>
       </c>
     </row>
@@ -1611,462 +2079,693 @@
         <v>7</v>
       </c>
       <c r="B16">
+        <f t="shared" si="5"/>
+        <v>43</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="6"/>
+        <v>118.32541950002913</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="7"/>
+        <v>146</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="F16">
         <f t="shared" si="3"/>
-        <v>43</v>
-      </c>
-      <c r="C16">
+        <v>0.36340458526740665</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="4"/>
-        <v>118.32541950002913</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="5"/>
-        <v>146</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="6"/>
+        <v>0.29452054794520549</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17">
+        <f>AVERAGE(E11:E16)</f>
         <v>1</v>
       </c>
-      <c r="F16">
-        <f>B16/C16</f>
-        <v>0.36340458526740665</v>
-      </c>
-      <c r="G16">
-        <f>B16/D16</f>
-        <v>0.29452054794520549</v>
+      <c r="F17">
+        <f>AVERAGE(F11:F16)</f>
+        <v>0.70746827108500243</v>
+      </c>
+      <c r="G17">
+        <f>AVERAGE(G11:G16)</f>
+        <v>0.50988851671181712</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <f>E30</f>
+        <v>1923</v>
+      </c>
+      <c r="C20">
+        <f>1000*1000*C48/B48</f>
+        <v>2021.0409745293466</v>
+      </c>
+      <c r="D20">
+        <f>E39</f>
+        <v>2403</v>
+      </c>
+      <c r="E20">
+        <f>B20/B20</f>
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ref="F20:F25" si="9">B20/C20</f>
+        <v>0.95148986301369864</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20:G25" si="10">B20/D20</f>
+        <v>0.80024968789013728</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ref="B21:B25" si="11">E31</f>
+        <v>343</v>
+      </c>
+      <c r="C21">
+        <f t="shared" ref="C21:C25" si="12">1000*1000*C49/B49</f>
+        <v>368.45071971623793</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ref="D21:D25" si="13">E40</f>
+        <v>376</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ref="E21:E25" si="14">B21/B21</f>
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="9"/>
+        <v>0.9309250373134329</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="10"/>
+        <v>0.91223404255319152</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="11"/>
+        <v>5</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="12"/>
+        <v>6.6089628677309555</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="13"/>
+        <v>15</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="9"/>
+        <v>0.75654835714285706</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="10"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="12"/>
+        <v>2.3367404884817518</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="9"/>
+        <v>0.85589307407407411</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="10"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="11"/>
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="12"/>
+        <v>2.3632764736556142</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="13"/>
+        <v>8</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="9"/>
+        <v>0.84628270212765966</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="10"/>
+        <v>0.25</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="11"/>
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="12"/>
+        <v>14.566802400609035</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="13"/>
+        <v>22</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="9"/>
+        <v>0.89244019672131147</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="10"/>
+        <v>0.59090909090909094</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="s">
-        <v>13</v>
-      </c>
-      <c r="G26" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27">
-        <v>128401</v>
-      </c>
-      <c r="C27">
-        <v>7764</v>
-      </c>
-      <c r="D27">
-        <v>7827</v>
-      </c>
-      <c r="E27">
-        <v>1923</v>
-      </c>
-      <c r="F27">
-        <v>4.04</v>
-      </c>
-      <c r="G27">
-        <v>4.07</v>
+        <v>26</v>
+      </c>
+      <c r="E26">
+        <f>AVERAGE(E20:E25)</f>
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <f>AVERAGE(F20:F25)</f>
+        <v>0.8722632050655057</v>
+      </c>
+      <c r="G26">
+        <f>AVERAGE(G20:G25)</f>
+        <v>0.52278769244762546</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>3</v>
-      </c>
-      <c r="B28">
-        <v>771919</v>
-      </c>
-      <c r="C28">
-        <v>1291</v>
-      </c>
-      <c r="D28">
-        <v>1298</v>
-      </c>
-      <c r="E28">
-        <v>343</v>
-      </c>
-      <c r="F28">
-        <v>3.76</v>
-      </c>
-      <c r="G28">
-        <v>3.78</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>4</v>
-      </c>
-      <c r="B29">
-        <v>172782863</v>
-      </c>
-      <c r="C29">
-        <v>4</v>
-      </c>
-      <c r="D29">
-        <v>15</v>
-      </c>
-      <c r="E29">
-        <v>5</v>
-      </c>
-      <c r="F29">
-        <v>0.78</v>
-      </c>
-      <c r="G29">
-        <v>2.66</v>
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B30">
-        <v>248920118</v>
+        <v>128401</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>7764</v>
       </c>
       <c r="D30">
-        <v>9</v>
+        <v>7827</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>1923</v>
       </c>
       <c r="F30">
-        <v>2.0099999999999998</v>
+        <v>4.04</v>
       </c>
       <c r="G30">
-        <v>4.53</v>
+        <v>4.07</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B31">
-        <v>233991854</v>
+        <v>771919</v>
       </c>
       <c r="C31">
-        <v>4</v>
+        <v>1291</v>
       </c>
       <c r="D31">
-        <v>4</v>
+        <v>1298</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>343</v>
       </c>
       <c r="F31">
-        <v>1.98</v>
+        <v>3.76</v>
       </c>
       <c r="G31">
-        <v>1.96</v>
+        <v>3.78</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B32">
-        <v>25512798</v>
+        <v>172782863</v>
       </c>
       <c r="C32">
-        <v>38</v>
+        <v>4</v>
       </c>
       <c r="D32">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="E32">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F32">
-        <v>2.91</v>
+        <v>0.78</v>
       </c>
       <c r="G32">
-        <v>3.27</v>
+        <v>2.66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>248920118</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+      <c r="D33">
+        <v>9</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+      <c r="F33">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="G33">
+        <v>4.53</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>233991854</v>
+      </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>1.98</v>
+      </c>
+      <c r="G34">
+        <v>1.96</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35">
+        <v>25512798</v>
+      </c>
+      <c r="C35">
+        <v>38</v>
+      </c>
+      <c r="D35">
+        <v>43</v>
+      </c>
+      <c r="E35">
         <v>13</v>
       </c>
-      <c r="G35" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36">
-        <v>107365</v>
-      </c>
-      <c r="C36">
-        <v>9360</v>
-      </c>
-      <c r="D36">
-        <v>9332</v>
-      </c>
-      <c r="E36">
-        <v>2403</v>
-      </c>
-      <c r="F36">
-        <v>3.9</v>
-      </c>
-      <c r="G36">
-        <v>3.88</v>
+      <c r="F35">
+        <v>2.91</v>
+      </c>
+      <c r="G35">
+        <v>3.27</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37">
-        <v>544318</v>
-      </c>
-      <c r="C37">
-        <v>1829</v>
-      </c>
-      <c r="D37">
-        <v>1824</v>
-      </c>
-      <c r="E37">
-        <v>376</v>
-      </c>
-      <c r="F37">
-        <v>4.8600000000000003</v>
-      </c>
-      <c r="G37">
-        <v>4.84</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38">
-        <v>27740105</v>
-      </c>
-      <c r="C38">
-        <v>35</v>
-      </c>
-      <c r="D38">
-        <v>36</v>
-      </c>
-      <c r="E38">
-        <v>15</v>
-      </c>
-      <c r="F38">
-        <v>2.38</v>
-      </c>
-      <c r="G38">
-        <v>2.41</v>
+        <v>0</v>
+      </c>
+      <c r="B38" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B39">
-        <v>60262988</v>
+        <v>107365</v>
       </c>
       <c r="C39">
-        <v>16</v>
+        <v>9360</v>
       </c>
       <c r="D39">
-        <v>16</v>
+        <v>9332</v>
       </c>
       <c r="E39">
-        <v>8</v>
+        <v>2403</v>
       </c>
       <c r="F39">
-        <v>1.88</v>
+        <v>3.9</v>
       </c>
       <c r="G39">
-        <v>1.87</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B40">
-        <v>58497963</v>
+        <v>544318</v>
       </c>
       <c r="C40">
-        <v>16</v>
+        <v>1829</v>
       </c>
       <c r="D40">
-        <v>17</v>
+        <v>1824</v>
       </c>
       <c r="E40">
-        <v>8</v>
+        <v>376</v>
       </c>
       <c r="F40">
-        <v>2.06</v>
+        <v>4.8600000000000003</v>
       </c>
       <c r="G40">
-        <v>2.12</v>
+        <v>4.84</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B41">
-        <v>6999839</v>
+        <v>27740105</v>
       </c>
       <c r="C41">
-        <v>145</v>
+        <v>35</v>
       </c>
       <c r="D41">
-        <v>146</v>
+        <v>36</v>
       </c>
       <c r="E41">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F41">
-        <v>6.45</v>
+        <v>2.38</v>
       </c>
       <c r="G41">
-        <v>6.47</v>
+        <v>2.41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42">
+        <v>60262988</v>
+      </c>
+      <c r="C42">
+        <v>16</v>
+      </c>
+      <c r="D42">
+        <v>16</v>
+      </c>
+      <c r="E42">
+        <v>8</v>
+      </c>
+      <c r="F42">
+        <v>1.88</v>
+      </c>
+      <c r="G42">
+        <v>1.87</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43">
+        <v>58497963</v>
+      </c>
+      <c r="C43">
         <v>16</v>
+      </c>
+      <c r="D43">
+        <v>17</v>
+      </c>
+      <c r="E43">
+        <v>8</v>
+      </c>
+      <c r="F43">
+        <v>2.06</v>
+      </c>
+      <c r="G43">
+        <v>2.12</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>6999839</v>
+      </c>
+      <c r="C44">
+        <v>145</v>
+      </c>
+      <c r="D44">
+        <v>146</v>
+      </c>
+      <c r="E44">
         <v>22</v>
       </c>
-      <c r="D44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>2</v>
-      </c>
-      <c r="B45">
-        <v>108360</v>
-      </c>
-      <c r="C45">
-        <v>219</v>
-      </c>
-      <c r="D45">
-        <v>844</v>
+      <c r="F44">
+        <v>6.45</v>
+      </c>
+      <c r="G44">
+        <v>6.47</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46">
-        <v>727370</v>
-      </c>
-      <c r="C46">
-        <v>268</v>
-      </c>
-      <c r="D46">
-        <v>1003</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>18</v>
-      </c>
-      <c r="B47">
-        <v>31775031</v>
-      </c>
-      <c r="C47">
-        <v>210</v>
-      </c>
-      <c r="D47">
-        <v>1011</v>
+        <v>0</v>
+      </c>
+      <c r="B47" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="B48">
-        <v>115545565</v>
+        <v>108360</v>
       </c>
       <c r="C48">
-        <v>270</v>
+        <v>219</v>
       </c>
       <c r="D48">
-        <v>1040</v>
+        <v>844</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B49">
-        <v>119325861</v>
+        <v>727370</v>
       </c>
       <c r="C49">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="D49">
-        <v>1029</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>18</v>
+      </c>
+      <c r="B50">
+        <v>31775031</v>
+      </c>
+      <c r="C50">
+        <v>210</v>
+      </c>
+      <c r="D50">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51">
+        <v>115545565</v>
+      </c>
+      <c r="C51">
+        <v>270</v>
+      </c>
+      <c r="D51">
+        <v>1040</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>20</v>
+      </c>
+      <c r="B52">
+        <v>119325861</v>
+      </c>
+      <c r="C52">
+        <v>282</v>
+      </c>
+      <c r="D52">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>21</v>
       </c>
-      <c r="B50">
+      <c r="B53">
         <v>8375208</v>
       </c>
-      <c r="C50">
+      <c r="C53">
         <v>122</v>
       </c>
-      <c r="D50">
+      <c r="D53">
         <v>991</v>
       </c>
     </row>

</xml_diff>